<commit_message>
from point to commma
</commit_message>
<xml_diff>
--- a/prioritization/rankings-of-compiled-circuits.xlsx
+++ b/prioritization/rankings-of-compiled-circuits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariesalm/Documents/PlanQK/Code/nisq-analyzer-content/prioritization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69033E74-E0FD-474F-83EC-8BAF279E76ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1898D75E-B13F-404F-B82E-5039D2D59C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8740" yWindow="29300" windowWidth="33600" windowHeight="20500" xr2:uid="{9395AFE9-CE9B-DA4A-ACC0-E0A9EA3F737D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>qpu name</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>bv-00110</t>
-  </si>
-  <si>
-    <t>99999.0</t>
   </si>
   <si>
     <t>TOP-C-Q-50</t>
@@ -708,10 +705,10 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,10 +753,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -810,34 +807,34 @@
         <v>17</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -851,7 +848,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>8192</v>
@@ -895,11 +892,11 @@
       <c r="R2" s="1">
         <v>0</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>30</v>
+      <c r="S2" s="1">
+        <v>99999</v>
+      </c>
+      <c r="T2" s="1">
+        <v>99999</v>
       </c>
       <c r="U2">
         <v>2</v>
@@ -946,7 +943,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3">
         <v>8192</v>
@@ -1041,7 +1038,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>8192</v>
@@ -1136,7 +1133,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>8192</v>
@@ -1231,7 +1228,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>8192</v>
@@ -1326,7 +1323,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>8192</v>
@@ -1421,7 +1418,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>8192</v>
@@ -1516,7 +1513,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>8192</v>
@@ -1560,11 +1557,11 @@
       <c r="R9" s="1">
         <v>0</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>30</v>
+      <c r="S9" s="1">
+        <v>99999</v>
+      </c>
+      <c r="T9" s="1">
+        <v>99999</v>
       </c>
       <c r="U9">
         <v>2</v>
@@ -1611,7 +1608,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>8192</v>
@@ -1706,7 +1703,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>8192</v>
@@ -1801,7 +1798,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>8192</v>
@@ -1896,7 +1893,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13">
         <v>8192</v>
@@ -1991,7 +1988,7 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>8192</v>
@@ -2086,7 +2083,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15">
         <v>8192</v>
@@ -2181,7 +2178,7 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16">
         <v>8192</v>
@@ -2225,11 +2222,11 @@
       <c r="R16" s="1">
         <v>0</v>
       </c>
-      <c r="S16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>30</v>
+      <c r="S16" s="1">
+        <v>99999</v>
+      </c>
+      <c r="T16" s="1">
+        <v>99999</v>
       </c>
       <c r="U16">
         <v>2</v>
@@ -2276,7 +2273,7 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17">
         <v>8192</v>
@@ -2371,7 +2368,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18">
         <v>8192</v>
@@ -2466,7 +2463,7 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19">
         <v>8192</v>
@@ -2561,7 +2558,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20">
         <v>8192</v>
@@ -2656,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>8192</v>
@@ -2751,7 +2748,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22">
         <v>8192</v>
@@ -3157,7 +3154,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="3:22" x14ac:dyDescent="0.2">

</xml_diff>